<commit_message>
added sdp to asn
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Auto\duAutomationPOC2\duAutomationPOC2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DU Automation\ASNConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
   <si>
     <t>Type</t>
   </si>
@@ -120,121 +120,118 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Parameter7</t>
-  </si>
-  <si>
-    <t>Parameter8</t>
-  </si>
-  <si>
-    <t>Parameter9</t>
-  </si>
-  <si>
-    <t>Parameter10</t>
-  </si>
-  <si>
-    <t>Parameter11</t>
-  </si>
-  <si>
-    <t>Parameter12</t>
-  </si>
-  <si>
-    <t>Parameter13</t>
-  </si>
-  <si>
-    <t>Parameter14</t>
-  </si>
-  <si>
-    <t>Parameter15</t>
-  </si>
-  <si>
-    <t>Parameter16</t>
-  </si>
-  <si>
-    <t>Parameter17</t>
-  </si>
-  <si>
-    <t>Parameter18</t>
-  </si>
-  <si>
-    <t>Parameter19</t>
-  </si>
-  <si>
-    <t>Parameter20</t>
-  </si>
-  <si>
-    <t>Parameter21</t>
-  </si>
-  <si>
-    <t>Parameter22</t>
-  </si>
-  <si>
-    <t>Parameter23</t>
-  </si>
-  <si>
-    <t>Parameter24</t>
-  </si>
-  <si>
-    <t>Parameter25</t>
-  </si>
-  <si>
-    <t>Parameter26</t>
-  </si>
-  <si>
-    <t>Parameter27</t>
-  </si>
-  <si>
-    <t>Parameter28</t>
-  </si>
-  <si>
-    <t>Parameter29</t>
-  </si>
-  <si>
-    <t>Parameter30</t>
-  </si>
-  <si>
-    <t>Parameter31</t>
-  </si>
-  <si>
-    <t>Parameter32</t>
-  </si>
-  <si>
-    <t>Parameter33</t>
-  </si>
-  <si>
-    <t>Parameter34</t>
-  </si>
-  <si>
-    <t>Parameter35</t>
-  </si>
-  <si>
-    <t>Parameter36</t>
-  </si>
-  <si>
-    <t>Parameter37</t>
-  </si>
-  <si>
-    <t>Parameter38</t>
-  </si>
-  <si>
-    <t>Parameter39</t>
-  </si>
-  <si>
-    <t>Parameter40</t>
-  </si>
-  <si>
-    <t>Parameter41</t>
-  </si>
-  <si>
-    <t>Parameter42</t>
-  </si>
-  <si>
-    <t>Parameter43</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>resultcode</t>
+    <t>value</t>
+  </si>
+  <si>
+    <t>triggerTime</t>
+  </si>
+  <si>
+    <t>nodeName</t>
+  </si>
+  <si>
+    <t>serviceContextID</t>
+  </si>
+  <si>
+    <t>chargingContextID</t>
+  </si>
+  <si>
+    <t>serviceSessionID</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>resultCode</t>
+  </si>
+  <si>
+    <t>recordIdentificationNumber</t>
+  </si>
+  <si>
+    <t>partialSequenceNumber</t>
+  </si>
+  <si>
+    <t>lastPartialOutput</t>
+  </si>
+  <si>
+    <t>subscriptionIDType</t>
+  </si>
+  <si>
+    <t>subscriptionIDValue</t>
+  </si>
+  <si>
+    <t>sessionId</t>
+  </si>
+  <si>
+    <t>ccRequestNumber</t>
+  </si>
+  <si>
+    <t>originRealm</t>
+  </si>
+  <si>
+    <t>originHost</t>
+  </si>
+  <si>
+    <t>serviceIdentifier</t>
+  </si>
+  <si>
+    <t>tariffChangeUsage</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>decimals</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>eventTime</t>
+  </si>
+  <si>
+    <t>serviceScenario</t>
+  </si>
+  <si>
+    <t>roamingPosition</t>
+  </si>
+  <si>
+    <t>servedAccount</t>
+  </si>
+  <si>
+    <t>serviceClassID</t>
+  </si>
+  <si>
+    <t>accountGroupID</t>
+  </si>
+  <si>
+    <t>amount[1]</t>
+  </si>
+  <si>
+    <t>decimals[1]</t>
+  </si>
+  <si>
+    <t>currency[1]</t>
+  </si>
+  <si>
+    <t>accountValueAfter</t>
+  </si>
+  <si>
+    <t>value3</t>
+  </si>
+  <si>
+    <t>value4</t>
+  </si>
+  <si>
+    <t>value5</t>
+  </si>
+  <si>
+    <t>value6</t>
   </si>
 </sst>
 </file>
@@ -552,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT5"/>
+  <dimension ref="A1:BO5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,29 +561,34 @@
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -600,133 +602,43 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" t="s">
-        <v>42</v>
-      </c>
-      <c r="V1" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>67</v>
-      </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -739,20 +651,20 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -765,13 +677,13 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -783,21 +695,36 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
         <v>20</v>
       </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
@@ -806,7 +733,196 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" t="s">
+        <v>44</v>
+      </c>
+      <c r="W5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>29</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>61</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>62</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change after delete file cdr
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="172">
   <si>
     <t>Type</t>
   </si>
@@ -117,15 +117,9 @@
     <t>accountValueBefore</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>triggerTime</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>value2</t>
   </si>
   <si>
-    <t>resultCode</t>
-  </si>
-  <si>
     <t>recordIdentificationNumber</t>
   </si>
   <si>
@@ -232,16 +223,348 @@
   </si>
   <si>
     <t>value6</t>
+  </si>
+  <si>
+    <t>Parameter7</t>
+  </si>
+  <si>
+    <t>value7</t>
+  </si>
+  <si>
+    <t>Parameter8</t>
+  </si>
+  <si>
+    <t>value8</t>
+  </si>
+  <si>
+    <t>Parameter9</t>
+  </si>
+  <si>
+    <t>value9</t>
+  </si>
+  <si>
+    <t>Parameter10</t>
+  </si>
+  <si>
+    <t>value10</t>
+  </si>
+  <si>
+    <t>Parameter11</t>
+  </si>
+  <si>
+    <t>value11</t>
+  </si>
+  <si>
+    <t>Parameter12</t>
+  </si>
+  <si>
+    <t>value12</t>
+  </si>
+  <si>
+    <t>Parameter13</t>
+  </si>
+  <si>
+    <t>value13</t>
+  </si>
+  <si>
+    <t>Parameter14</t>
+  </si>
+  <si>
+    <t>value14</t>
+  </si>
+  <si>
+    <t>Parameter15</t>
+  </si>
+  <si>
+    <t>value15</t>
+  </si>
+  <si>
+    <t>Parameter16</t>
+  </si>
+  <si>
+    <t>value16</t>
+  </si>
+  <si>
+    <t>Parameter17</t>
+  </si>
+  <si>
+    <t>value17</t>
+  </si>
+  <si>
+    <t>Parameter18</t>
+  </si>
+  <si>
+    <t>value18</t>
+  </si>
+  <si>
+    <t>Parameter19</t>
+  </si>
+  <si>
+    <t>value19</t>
+  </si>
+  <si>
+    <t>Parameter20</t>
+  </si>
+  <si>
+    <t>value20</t>
+  </si>
+  <si>
+    <t>Parameter21</t>
+  </si>
+  <si>
+    <t>value21</t>
+  </si>
+  <si>
+    <t>Parameter22</t>
+  </si>
+  <si>
+    <t>value22</t>
+  </si>
+  <si>
+    <t>Parameter23</t>
+  </si>
+  <si>
+    <t>value23</t>
+  </si>
+  <si>
+    <t>Parameter24</t>
+  </si>
+  <si>
+    <t>value24</t>
+  </si>
+  <si>
+    <t>Parameter25</t>
+  </si>
+  <si>
+    <t>value25</t>
+  </si>
+  <si>
+    <t>Parameter26</t>
+  </si>
+  <si>
+    <t>value26</t>
+  </si>
+  <si>
+    <t>Parameter27</t>
+  </si>
+  <si>
+    <t>value27</t>
+  </si>
+  <si>
+    <t>Parameter28</t>
+  </si>
+  <si>
+    <t>value28</t>
+  </si>
+  <si>
+    <t>Parameter29</t>
+  </si>
+  <si>
+    <t>value29</t>
+  </si>
+  <si>
+    <t>Parameter30</t>
+  </si>
+  <si>
+    <t>value30</t>
+  </si>
+  <si>
+    <t>Parameter31</t>
+  </si>
+  <si>
+    <t>value31</t>
+  </si>
+  <si>
+    <t>Parameter32</t>
+  </si>
+  <si>
+    <t>value32</t>
+  </si>
+  <si>
+    <t>Parameter33</t>
+  </si>
+  <si>
+    <t>value33</t>
+  </si>
+  <si>
+    <t>More Time Recharge</t>
+  </si>
+  <si>
+    <t>originTimeStamp</t>
+  </si>
+  <si>
+    <t>subscriberNumber</t>
+  </si>
+  <si>
+    <t>accountInformationBeforeRefill</t>
+  </si>
+  <si>
+    <t>permanentServiceClass</t>
+  </si>
+  <si>
+    <t>accountInformationAfterRefill</t>
+  </si>
+  <si>
+    <t>treeDefinedFields</t>
+  </si>
+  <si>
+    <t>externalData</t>
+  </si>
+  <si>
+    <t>externalData2</t>
+  </si>
+  <si>
+    <t>externalData3</t>
+  </si>
+  <si>
+    <t>adjustmentRecordType[0]</t>
+  </si>
+  <si>
+    <t>sdpID[0]</t>
+  </si>
+  <si>
+    <t>cdrID[0]</t>
+  </si>
+  <si>
+    <t>accountNumber[0]</t>
+  </si>
+  <si>
+    <t>subscriberNumber[0]</t>
+  </si>
+  <si>
+    <t>adjustmentTimeStamp[0]</t>
+  </si>
+  <si>
+    <t>serviceClassId[0]</t>
+  </si>
+  <si>
+    <t>currencyType[0]</t>
+  </si>
+  <si>
+    <t>originNodeType[0]</t>
+  </si>
+  <si>
+    <t>originNodeId[0]</t>
+  </si>
+  <si>
+    <t>origTransactionID[0]</t>
+  </si>
+  <si>
+    <t>origTransactionTimeStamp[0]</t>
+  </si>
+  <si>
+    <t>originOperatorId[0]</t>
+  </si>
+  <si>
+    <t>accountFlagsBefore[0]</t>
+  </si>
+  <si>
+    <t>accountFlagsAfter[0]</t>
+  </si>
+  <si>
+    <t>activationDate[0]</t>
+  </si>
+  <si>
+    <t>offerID[0]</t>
+  </si>
+  <si>
+    <t>action[0]</t>
+  </si>
+  <si>
+    <t>offerType[0]</t>
+  </si>
+  <si>
+    <t>offerDisabledAfter[0]</t>
+  </si>
+  <si>
+    <t>Parameter34</t>
+  </si>
+  <si>
+    <t>value34</t>
+  </si>
+  <si>
+    <t>Parameter35</t>
+  </si>
+  <si>
+    <t>value35</t>
+  </si>
+  <si>
+    <t>Parameter36</t>
+  </si>
+  <si>
+    <t>value36</t>
+  </si>
+  <si>
+    <t>Parameter37</t>
+  </si>
+  <si>
+    <t>value37</t>
+  </si>
+  <si>
+    <t>Parameter38</t>
+  </si>
+  <si>
+    <t>value38</t>
+  </si>
+  <si>
+    <t>Parameter39</t>
+  </si>
+  <si>
+    <t>value39</t>
+  </si>
+  <si>
+    <t>Parameter40</t>
+  </si>
+  <si>
+    <t>value40</t>
+  </si>
+  <si>
+    <t>value41</t>
+  </si>
+  <si>
+    <t>Parameter41</t>
+  </si>
+  <si>
+    <t>Parameter42</t>
+  </si>
+  <si>
+    <t>value42</t>
+  </si>
+  <si>
+    <t>Parameter43</t>
+  </si>
+  <si>
+    <t>value43</t>
+  </si>
+  <si>
+    <t>decimals[2]</t>
+  </si>
+  <si>
+    <t>currency[2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF990000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,8 +590,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BO5"/>
+  <dimension ref="A1:CK5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +913,7 @@
     <col min="31" max="33" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -602,45 +927,264 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J1" t="s">
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
       </c>
       <c r="O1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" t="s">
-        <v>32</v>
+      <c r="S1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W1" t="s">
+        <v>73</v>
+      </c>
+      <c r="X1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>114</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>115</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>151</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>152</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>153</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>158</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>159</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>160</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>161</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>162</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>163</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>165</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>164</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>166</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>167</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>168</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -651,22 +1195,29 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -677,13 +1228,82 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>16</v>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="S3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="W3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -695,36 +1315,132 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>134</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" t="s">
+        <v>136</v>
+      </c>
+      <c r="S4" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" t="s">
+        <v>137</v>
+      </c>
+      <c r="U4" t="s">
+        <v>30</v>
+      </c>
+      <c r="V4" t="s">
+        <v>138</v>
+      </c>
+      <c r="W4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X4" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
@@ -733,196 +1449,214 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
+      <c r="U5" t="s">
+        <v>30</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" t="s">
+        <v>30</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>31</v>
-      </c>
-      <c r="R5" t="s">
-        <v>42</v>
-      </c>
-      <c r="S5" t="s">
-        <v>31</v>
-      </c>
-      <c r="T5" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" t="s">
-        <v>31</v>
-      </c>
-      <c r="V5" t="s">
-        <v>44</v>
-      </c>
-      <c r="W5" t="s">
-        <v>31</v>
-      </c>
-      <c r="X5" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN5" t="s">
+      <c r="AU5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AV5" t="s">
         <v>53</v>
       </c>
-      <c r="AO5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP5" t="s">
+      <c r="AW5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX5" t="s">
         <v>54</v>
       </c>
-      <c r="AQ5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR5" t="s">
+      <c r="AY5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AZ5" t="s">
         <v>55</v>
       </c>
-      <c r="AS5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AV5" t="s">
+      <c r="BA5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BB5" t="s">
         <v>56</v>
       </c>
-      <c r="AW5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX5" t="s">
+      <c r="BC5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BD5" t="s">
         <v>57</v>
       </c>
-      <c r="AY5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>31</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>31</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>60</v>
-      </c>
       <c r="BE5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BF5" t="s">
         <v>29</v>
       </c>
       <c r="BG5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BH5" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BN5" t="s">
         <v>61</v>
       </c>
-      <c r="BI5" t="s">
-        <v>31</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>62</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>31</v>
-      </c>
-      <c r="BL5" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM5" t="s">
-        <v>31</v>
-      </c>
-      <c r="BN5" t="s">
-        <v>64</v>
-      </c>
       <c r="BO5" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="BP5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BQ5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>170</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>171</v>
+      </c>
+      <c r="BU5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -935,6 +1669,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
EDR file and time stamp change
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="225">
   <si>
     <t>Type</t>
   </si>
@@ -201,15 +201,6 @@
     <t>accountGroupID</t>
   </si>
   <si>
-    <t>amount[1]</t>
-  </si>
-  <si>
-    <t>decimals[1]</t>
-  </si>
-  <si>
-    <t>currency[1]</t>
-  </si>
-  <si>
     <t>accountValueAfter</t>
   </si>
   <si>
@@ -537,10 +528,178 @@
     <t>value43</t>
   </si>
   <si>
-    <t>decimals[2]</t>
-  </si>
-  <si>
-    <t>currency[2]</t>
+    <t>Parameter44</t>
+  </si>
+  <si>
+    <t>value44</t>
+  </si>
+  <si>
+    <t>Parameter45</t>
+  </si>
+  <si>
+    <t>value45</t>
+  </si>
+  <si>
+    <t>Parameter46</t>
+  </si>
+  <si>
+    <t>value46</t>
+  </si>
+  <si>
+    <t>Parameter47</t>
+  </si>
+  <si>
+    <t>value47</t>
+  </si>
+  <si>
+    <t>Parameter48</t>
+  </si>
+  <si>
+    <t>value48</t>
+  </si>
+  <si>
+    <t>Parameter49</t>
+  </si>
+  <si>
+    <t>value49</t>
+  </si>
+  <si>
+    <t>Parameter50</t>
+  </si>
+  <si>
+    <t>value50</t>
+  </si>
+  <si>
+    <t>Parameter51</t>
+  </si>
+  <si>
+    <t>value51</t>
+  </si>
+  <si>
+    <t>Parameter52</t>
+  </si>
+  <si>
+    <t>value52</t>
+  </si>
+  <si>
+    <t>Parameter53</t>
+  </si>
+  <si>
+    <t>value53</t>
+  </si>
+  <si>
+    <t>Parameter54</t>
+  </si>
+  <si>
+    <t>value54</t>
+  </si>
+  <si>
+    <t>Parameter55</t>
+  </si>
+  <si>
+    <t>value55</t>
+  </si>
+  <si>
+    <t>Parameter56</t>
+  </si>
+  <si>
+    <t>value56</t>
+  </si>
+  <si>
+    <t>Parameter57</t>
+  </si>
+  <si>
+    <t>value57</t>
+  </si>
+  <si>
+    <t>Parameter58</t>
+  </si>
+  <si>
+    <t>value58</t>
+  </si>
+  <si>
+    <t>Parameter59</t>
+  </si>
+  <si>
+    <t>value59</t>
+  </si>
+  <si>
+    <t>Parameter60</t>
+  </si>
+  <si>
+    <t>value60</t>
+  </si>
+  <si>
+    <t>Parameter61</t>
+  </si>
+  <si>
+    <t>value61</t>
+  </si>
+  <si>
+    <t>Parameter62</t>
+  </si>
+  <si>
+    <t>value62</t>
+  </si>
+  <si>
+    <t>Parameter63</t>
+  </si>
+  <si>
+    <t>value63</t>
+  </si>
+  <si>
+    <t>Parameter64</t>
+  </si>
+  <si>
+    <t>value64</t>
+  </si>
+  <si>
+    <t>Parameter65</t>
+  </si>
+  <si>
+    <t>value65</t>
+  </si>
+  <si>
+    <t>Parameter66</t>
+  </si>
+  <si>
+    <t>value66</t>
+  </si>
+  <si>
+    <t>Parameter67</t>
+  </si>
+  <si>
+    <t>value67</t>
+  </si>
+  <si>
+    <t>Parameter68</t>
+  </si>
+  <si>
+    <t>value68</t>
+  </si>
+  <si>
+    <t>Parameter69</t>
+  </si>
+  <si>
+    <t>value69</t>
+  </si>
+  <si>
+    <t>Parameter70</t>
+  </si>
+  <si>
+    <t>value70</t>
+  </si>
+  <si>
+    <t>Parameter71</t>
+  </si>
+  <si>
+    <t>value71</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>CIS</t>
   </si>
 </sst>
 </file>
@@ -874,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK5"/>
+  <dimension ref="A1:EO6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +1072,7 @@
     <col min="31" max="33" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -939,250 +1098,418 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J1" t="s">
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
       </c>
       <c r="O1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" t="s">
         <v>65</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>67</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>68</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>69</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>70</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>71</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>72</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>73</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>74</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>78</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>79</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>80</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>81</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>82</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>83</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>85</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>86</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>87</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>88</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>89</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>90</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>91</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>92</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>93</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>94</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>95</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>96</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>97</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>98</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>99</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>100</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>101</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>102</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>103</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>104</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>105</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>106</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
         <v>107</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BI1" t="s">
         <v>108</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BJ1" t="s">
         <v>109</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BK1" t="s">
         <v>110</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BL1" t="s">
         <v>111</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BM1" t="s">
         <v>112</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BN1" t="s">
         <v>113</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BO1" t="s">
         <v>114</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BP1" t="s">
         <v>115</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BQ1" t="s">
         <v>116</v>
       </c>
-      <c r="BO1" t="s">
-        <v>117</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>119</v>
-      </c>
       <c r="BR1" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BU1" t="s">
         <v>150</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BV1" t="s">
         <v>151</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BW1" t="s">
         <v>152</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BX1" t="s">
         <v>153</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BY1" t="s">
         <v>154</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BZ1" t="s">
         <v>155</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CA1" t="s">
         <v>156</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CB1" t="s">
         <v>157</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CC1" t="s">
         <v>158</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CD1" t="s">
         <v>159</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CE1" t="s">
         <v>160</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CF1" t="s">
+        <v>162</v>
+      </c>
+      <c r="CG1" t="s">
         <v>161</v>
       </c>
-      <c r="CD1" t="s">
-        <v>162</v>
-      </c>
-      <c r="CE1" t="s">
+      <c r="CH1" t="s">
         <v>163</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CI1" t="s">
+        <v>164</v>
+      </c>
+      <c r="CJ1" t="s">
         <v>165</v>
       </c>
-      <c r="CG1" t="s">
-        <v>164</v>
-      </c>
-      <c r="CH1" t="s">
+      <c r="CK1" t="s">
         <v>166</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CL1" t="s">
         <v>167</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CM1" t="s">
         <v>168</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CN1" t="s">
         <v>169</v>
       </c>
+      <c r="CO1" t="s">
+        <v>170</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>171</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>172</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>173</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>174</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>175</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>176</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>177</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>178</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>179</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>180</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>181</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>182</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>183</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>184</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>185</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>186</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>187</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>188</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>189</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>190</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>191</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>192</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>193</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>194</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>195</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>196</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>197</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>198</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>199</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>200</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>202</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>203</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>204</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>205</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>206</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>207</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>208</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>209</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>210</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>211</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>212</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>213</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>214</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>215</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>216</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>217</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>218</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>219</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>220</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>221</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>222</v>
+      </c>
     </row>
-    <row r="2" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1193,7 +1520,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
@@ -1215,7 +1542,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1232,62 +1559,62 @@
         <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="S3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="O3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="Q3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="2" t="s">
+      <c r="W3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="S3" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="U3" t="s">
-        <v>30</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="W3" t="s">
-        <v>30</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="Y3" t="s">
         <v>30</v>
       </c>
@@ -1301,7 +1628,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1318,127 +1645,127 @@
         <v>30</v>
       </c>
       <c r="F4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>129</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" t="s">
         <v>130</v>
       </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
         <v>131</v>
       </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
         <v>132</v>
       </c>
-      <c r="K4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="Q4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" t="s">
         <v>133</v>
       </c>
-      <c r="M4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="S4" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" t="s">
         <v>134</v>
       </c>
-      <c r="O4" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="U4" t="s">
+        <v>30</v>
+      </c>
+      <c r="V4" t="s">
         <v>135</v>
       </c>
-      <c r="Q4" t="s">
-        <v>30</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="W4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X4" t="s">
         <v>136</v>
       </c>
-      <c r="S4" t="s">
-        <v>30</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="Y4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z4" t="s">
         <v>137</v>
       </c>
-      <c r="U4" t="s">
-        <v>30</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="AA4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB4" t="s">
         <v>138</v>
       </c>
-      <c r="W4" t="s">
-        <v>30</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="AC4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD4" t="s">
         <v>139</v>
       </c>
-      <c r="Y4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="AE4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF4" t="s">
         <v>140</v>
       </c>
-      <c r="AA4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB4" t="s">
+      <c r="AG4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH4" t="s">
         <v>141</v>
       </c>
-      <c r="AC4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD4" t="s">
+      <c r="AI4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>142</v>
       </c>
-      <c r="AE4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF4" t="s">
+      <c r="AK4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL4" t="s">
         <v>143</v>
       </c>
-      <c r="AG4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH4" t="s">
+      <c r="AM4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN4" t="s">
         <v>144</v>
       </c>
-      <c r="AI4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ4" t="s">
+      <c r="AO4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP4" t="s">
         <v>145</v>
       </c>
-      <c r="AK4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL4" t="s">
+      <c r="AQ4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AR4" t="s">
         <v>146</v>
       </c>
-      <c r="AM4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>147</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>148</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>149</v>
-      </c>
       <c r="AS4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1449,7 +1776,7 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
@@ -1617,46 +1944,267 @@
         <v>30</v>
       </c>
       <c r="BH5" t="s">
+        <v>49</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BN5" t="s">
         <v>58</v>
       </c>
-      <c r="BI5" t="s">
-        <v>30</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>59</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>30</v>
-      </c>
-      <c r="BL5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BM5" t="s">
-        <v>30</v>
-      </c>
-      <c r="BN5" t="s">
-        <v>61</v>
-      </c>
       <c r="BO5" t="s">
         <v>30</v>
       </c>
       <c r="BP5" s="2" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="BQ5" t="s">
         <v>30</v>
       </c>
       <c r="BR5" t="s">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="BS5" t="s">
         <v>30</v>
       </c>
       <c r="BT5" t="s">
-        <v>171</v>
+        <v>51</v>
       </c>
       <c r="BU5" t="s">
         <v>30</v>
+      </c>
+      <c r="BV5" t="s">
+        <v>42</v>
+      </c>
+      <c r="BW5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BX5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>32</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CB5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="CC5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CD5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="CE5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CF5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="CG5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CH5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="CI5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CJ5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="CK5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CL5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CN5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="CO5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CP5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="CQ5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CR5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="CS5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CT5" t="s">
+        <v>44</v>
+      </c>
+      <c r="CU5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CV5" t="s">
+        <v>45</v>
+      </c>
+      <c r="CW5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CX5" t="s">
+        <v>46</v>
+      </c>
+      <c r="CY5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CZ5" t="s">
+        <v>47</v>
+      </c>
+      <c r="DA5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DB5" t="s">
+        <v>48</v>
+      </c>
+      <c r="DC5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DD5" t="s">
+        <v>49</v>
+      </c>
+      <c r="DE5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DF5" t="s">
+        <v>50</v>
+      </c>
+      <c r="DG5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DH5" t="s">
+        <v>51</v>
+      </c>
+      <c r="DI5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DJ5" t="s">
+        <v>52</v>
+      </c>
+      <c r="DK5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DL5" t="s">
+        <v>31</v>
+      </c>
+      <c r="DM5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DN5" t="s">
+        <v>53</v>
+      </c>
+      <c r="DO5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DP5" t="s">
+        <v>54</v>
+      </c>
+      <c r="DQ5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DR5" t="s">
+        <v>55</v>
+      </c>
+      <c r="DS5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DT5" t="s">
+        <v>56</v>
+      </c>
+      <c r="DU5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DV5" t="s">
+        <v>57</v>
+      </c>
+      <c r="DW5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DX5" t="s">
+        <v>29</v>
+      </c>
+      <c r="DY5" t="s">
+        <v>30</v>
+      </c>
+      <c r="DZ5" t="s">
+        <v>49</v>
+      </c>
+      <c r="EA5" t="s">
+        <v>30</v>
+      </c>
+      <c r="EB5" t="s">
+        <v>50</v>
+      </c>
+      <c r="EC5" t="s">
+        <v>30</v>
+      </c>
+      <c r="ED5" t="s">
+        <v>51</v>
+      </c>
+      <c r="EE5" t="s">
+        <v>30</v>
+      </c>
+      <c r="EF5" t="s">
+        <v>58</v>
+      </c>
+      <c r="EG5" t="s">
+        <v>30</v>
+      </c>
+      <c r="EH5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="EI5" t="s">
+        <v>30</v>
+      </c>
+      <c r="EJ5" t="s">
+        <v>50</v>
+      </c>
+      <c r="EK5" t="s">
+        <v>30</v>
+      </c>
+      <c r="EL5" t="s">
+        <v>51</v>
+      </c>
+      <c r="EM5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:145" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>